<commit_message>
Revised data file - improved names of columns
</commit_message>
<xml_diff>
--- a/data/quiz/grades_h19.xlsx
+++ b/data/quiz/grades_h19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\M221R\data\quiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D54DB008-D62A-46A8-9F33-678487B45FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7E1352-C16B-4FC3-862D-F286C34B686D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-8205" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="16">
   <si>
     <t>grade</t>
-  </si>
-  <si>
-    <t>name</t>
   </si>
   <si>
     <t>A</t>
@@ -80,6 +77,9 @@
   </si>
   <si>
     <t>Online</t>
+  </si>
+  <si>
+    <t>course_type</t>
   </si>
 </sst>
 </file>
@@ -472,22 +472,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="10.54296875" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" customWidth="1"/>
     <col min="4" max="4" width="29.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -495,13 +497,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -509,13 +511,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -523,10 +525,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -534,13 +536,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -548,13 +550,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -562,13 +564,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -576,10 +578,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -587,10 +589,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -598,10 +600,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -609,10 +611,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -620,10 +622,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -631,10 +633,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -642,10 +644,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -653,10 +655,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -664,10 +666,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -675,10 +677,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -686,10 +688,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -697,10 +699,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -708,10 +710,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -719,10 +721,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -730,10 +732,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -741,10 +743,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -752,10 +754,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -763,10 +765,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -774,10 +776,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -785,10 +787,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -796,10 +798,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -807,10 +809,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -818,10 +820,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -829,10 +831,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -840,10 +842,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -851,10 +853,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C33" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -862,10 +864,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -873,10 +875,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -884,10 +886,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -895,10 +897,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -906,10 +908,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -917,10 +919,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -928,10 +930,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
@@ -939,10 +941,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -950,10 +952,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C42" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -961,10 +963,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C43" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -972,10 +974,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C44" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -983,10 +985,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -994,10 +996,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C46" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
@@ -1005,10 +1007,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C47" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -1016,10 +1018,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C48" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -1027,10 +1029,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C49" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -1038,10 +1040,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C50" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -1049,10 +1051,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C51" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -1060,10 +1062,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C52" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
@@ -1071,10 +1073,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C53" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -1082,10 +1084,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C54" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -1093,10 +1095,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C55" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -1104,10 +1106,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C56" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
@@ -1115,10 +1117,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C57" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
@@ -1126,10 +1128,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C58" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
@@ -1137,10 +1139,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C59" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -1148,10 +1150,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C60" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
@@ -1159,10 +1161,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C61" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
@@ -1170,10 +1172,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C62" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
@@ -1181,10 +1183,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C63" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -1192,10 +1194,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C64" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
@@ -1203,10 +1205,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C65" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
@@ -1214,10 +1216,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C66" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
@@ -1225,10 +1227,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C67" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
@@ -1236,10 +1238,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C68" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
@@ -1247,10 +1249,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C69" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -1258,10 +1260,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C70" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
@@ -1269,10 +1271,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C71" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
@@ -1280,10 +1282,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C72" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
@@ -1291,10 +1293,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C73" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -1302,10 +1304,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C74" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
@@ -1313,10 +1315,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C75" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
@@ -1324,10 +1326,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C76" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
@@ -1335,10 +1337,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C77" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -1346,10 +1348,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C78" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -1357,10 +1359,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C79" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -1368,10 +1370,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C80" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
@@ -1379,10 +1381,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C81" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
@@ -1390,10 +1392,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C82" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
@@ -1401,10 +1403,10 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C83" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -1412,10 +1414,10 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C84" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
@@ -1423,10 +1425,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C85" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -1434,10 +1436,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C86" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
@@ -1445,10 +1447,10 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C87" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
@@ -1456,10 +1458,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C88" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
@@ -1467,10 +1469,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C89" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
@@ -1478,10 +1480,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C90" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
@@ -1489,10 +1491,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C91" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
@@ -1500,10 +1502,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C92" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
@@ -1511,10 +1513,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C93" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
@@ -1522,10 +1524,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C94" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -1533,10 +1535,10 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C95" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
@@ -1544,10 +1546,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C96" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
@@ -1555,10 +1557,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C97" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
@@ -1566,10 +1568,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C98" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
@@ -1577,10 +1579,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C99" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
@@ -1588,10 +1590,10 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C100" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
@@ -1599,10 +1601,10 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C101" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
@@ -1610,10 +1612,10 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C102" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
@@ -1621,10 +1623,10 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C103" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
@@ -1632,10 +1634,10 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C104" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
@@ -1643,10 +1645,10 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C105" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
@@ -1654,10 +1656,10 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C106" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
@@ -1665,10 +1667,10 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C107" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
@@ -1676,10 +1678,10 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C108" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
@@ -1687,10 +1689,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C109" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
@@ -1698,10 +1700,10 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C110" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
@@ -1709,10 +1711,10 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C111" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
@@ -1720,10 +1722,10 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C112" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
@@ -1731,10 +1733,10 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C113" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
@@ -1742,10 +1744,10 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C114" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
@@ -1753,10 +1755,10 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C115" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
@@ -1764,10 +1766,10 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C116" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
@@ -1775,10 +1777,10 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C117" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
@@ -1786,10 +1788,10 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C118" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
@@ -1797,10 +1799,10 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C119" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
@@ -1808,10 +1810,10 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C120" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
@@ -1819,10 +1821,10 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C121" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
@@ -1830,10 +1832,10 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C122" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
@@ -1841,10 +1843,10 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C123" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
@@ -1852,10 +1854,10 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C124" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
@@ -1863,10 +1865,10 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C125" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
@@ -1874,10 +1876,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C126" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
@@ -1885,10 +1887,10 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C127" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
@@ -1896,10 +1898,10 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C128" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
@@ -1907,10 +1909,10 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C129" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
@@ -1918,10 +1920,10 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C130" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
@@ -1929,10 +1931,10 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C131" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
@@ -1940,10 +1942,10 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C132" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
@@ -1951,10 +1953,10 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C133" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
@@ -1962,10 +1964,10 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C134" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
@@ -1973,10 +1975,10 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C135" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
@@ -1984,10 +1986,10 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C136" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
@@ -1995,10 +1997,10 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C137" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
@@ -2006,10 +2008,10 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C138" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
@@ -2017,10 +2019,10 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C139" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
@@ -2028,10 +2030,10 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C140" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
@@ -2039,10 +2041,10 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C141" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
@@ -2050,10 +2052,10 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C142" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
@@ -2061,10 +2063,10 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C143" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
@@ -2072,10 +2074,10 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C144" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
@@ -2083,10 +2085,10 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C145" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
@@ -2094,10 +2096,10 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C146" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
@@ -2105,10 +2107,10 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C147" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
@@ -2116,10 +2118,10 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C148" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
@@ -2127,10 +2129,10 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C149" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
@@ -2138,10 +2140,10 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C150" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
@@ -2149,10 +2151,10 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C151" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
@@ -2160,10 +2162,10 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C152" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
@@ -2171,10 +2173,10 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C153" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
@@ -2182,10 +2184,10 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C154" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
@@ -2193,10 +2195,10 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C155" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
@@ -2204,10 +2206,10 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C156" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
@@ -2215,10 +2217,10 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C157" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
@@ -2226,10 +2228,10 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C158" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
@@ -2237,10 +2239,10 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C159" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
@@ -2248,10 +2250,10 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C160" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
@@ -2259,10 +2261,10 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C161" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
@@ -2270,10 +2272,10 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C162" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
@@ -2281,10 +2283,10 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C163" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
@@ -2292,10 +2294,10 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C164" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
@@ -2303,10 +2305,10 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C165" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
@@ -2314,10 +2316,10 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C166" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
@@ -2325,10 +2327,10 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C167" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
@@ -2336,10 +2338,10 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C168" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
@@ -2347,10 +2349,10 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C169" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
@@ -2358,10 +2360,10 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C170" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
@@ -2369,10 +2371,10 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C171" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
@@ -2380,10 +2382,10 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C172" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
@@ -2391,10 +2393,10 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C173" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
@@ -2402,10 +2404,10 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C174" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
@@ -2413,10 +2415,10 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C175" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
@@ -2424,10 +2426,10 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C176" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
@@ -2435,10 +2437,10 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C177" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
@@ -2446,10 +2448,10 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C178" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
@@ -2457,10 +2459,10 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C179" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
@@ -2468,10 +2470,10 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C180" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.35">
@@ -2479,10 +2481,10 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C181" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
@@ -2490,10 +2492,10 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C182" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
@@ -2501,10 +2503,10 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C183" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
@@ -2512,10 +2514,10 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C184" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.35">
@@ -2523,10 +2525,10 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C185" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
@@ -2534,10 +2536,10 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C186" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
@@ -2545,10 +2547,10 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C187" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.35">
@@ -2556,10 +2558,10 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C188" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.35">
@@ -2567,10 +2569,10 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C189" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.35">
@@ -2578,10 +2580,10 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C190" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.35">
@@ -2589,10 +2591,10 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C191" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.35">
@@ -2600,10 +2602,10 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C192" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.35">
@@ -2611,10 +2613,10 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C193" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.35">
@@ -2622,10 +2624,10 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C194" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.35">
@@ -2633,10 +2635,10 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C195" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.35">
@@ -2644,10 +2646,10 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C196" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.35">
@@ -2655,10 +2657,10 @@
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C197" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.35">
@@ -2666,10 +2668,10 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C198" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.35">
@@ -2677,10 +2679,10 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C199" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.35">
@@ -2688,10 +2690,10 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C200" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.35">
@@ -2699,10 +2701,10 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C201" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.35">
@@ -2710,10 +2712,10 @@
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C202" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.35">
@@ -2721,10 +2723,10 @@
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C203" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.35">
@@ -2732,10 +2734,10 @@
         <v>203</v>
       </c>
       <c r="B204" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C204" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.35">
@@ -2743,10 +2745,10 @@
         <v>204</v>
       </c>
       <c r="B205" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C205" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.35">
@@ -2754,10 +2756,10 @@
         <v>205</v>
       </c>
       <c r="B206" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C206" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.35">
@@ -2765,10 +2767,10 @@
         <v>206</v>
       </c>
       <c r="B207" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C207" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.35">
@@ -2776,10 +2778,10 @@
         <v>207</v>
       </c>
       <c r="B208" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C208" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>